<commit_message>
Agregada la funcion para determinar las apuestas. Empezado el algoritmo para determinar las apuestas de todos los partidos de esa jornada
</commit_message>
<xml_diff>
--- a/DatosIng1/EP1213.xlsx
+++ b/DatosIng1/EP1213.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="142">
   <si>
     <t>Div</t>
   </si>
@@ -1262,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BR307"/>
+  <dimension ref="A1:BR317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
+      <selection activeCell="A316" sqref="A316:XFD317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -66336,6 +66336,2126 @@
         <v>1.66</v>
       </c>
     </row>
+    <row r="308" spans="1:70">
+      <c r="A308" t="s">
+        <v>70</v>
+      </c>
+      <c r="B308" s="1">
+        <v>41429</v>
+      </c>
+      <c r="C308" t="s">
+        <v>76</v>
+      </c>
+      <c r="D308" t="s">
+        <v>81</v>
+      </c>
+      <c r="E308">
+        <v>2</v>
+      </c>
+      <c r="F308">
+        <v>2</v>
+      </c>
+      <c r="G308" t="s">
+        <v>74</v>
+      </c>
+      <c r="H308">
+        <v>1</v>
+      </c>
+      <c r="I308">
+        <v>1</v>
+      </c>
+      <c r="J308" t="s">
+        <v>74</v>
+      </c>
+      <c r="K308">
+        <v>12</v>
+      </c>
+      <c r="L308">
+        <v>16</v>
+      </c>
+      <c r="M308">
+        <v>9</v>
+      </c>
+      <c r="N308">
+        <v>9</v>
+      </c>
+      <c r="O308">
+        <v>8</v>
+      </c>
+      <c r="P308">
+        <v>16</v>
+      </c>
+      <c r="Q308">
+        <v>2</v>
+      </c>
+      <c r="R308">
+        <v>5</v>
+      </c>
+      <c r="S308">
+        <v>5</v>
+      </c>
+      <c r="T308">
+        <v>3</v>
+      </c>
+      <c r="U308">
+        <v>0</v>
+      </c>
+      <c r="V308">
+        <v>0</v>
+      </c>
+      <c r="W308">
+        <v>2.63</v>
+      </c>
+      <c r="X308">
+        <v>3.3</v>
+      </c>
+      <c r="Y308">
+        <v>2.9</v>
+      </c>
+      <c r="Z308">
+        <v>2.6</v>
+      </c>
+      <c r="AA308">
+        <v>3.1</v>
+      </c>
+      <c r="AB308">
+        <v>2.8</v>
+      </c>
+      <c r="AC308">
+        <v>2.6</v>
+      </c>
+      <c r="AD308">
+        <v>3.1</v>
+      </c>
+      <c r="AE308">
+        <v>2.8</v>
+      </c>
+      <c r="AF308">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AG308">
+        <v>3.3</v>
+      </c>
+      <c r="AH308">
+        <v>2.9</v>
+      </c>
+      <c r="AI308">
+        <v>2.5</v>
+      </c>
+      <c r="AJ308">
+        <v>3.2</v>
+      </c>
+      <c r="AK308">
+        <v>2.8</v>
+      </c>
+      <c r="AL308">
+        <v>2.67</v>
+      </c>
+      <c r="AM308">
+        <v>3.33</v>
+      </c>
+      <c r="AN308">
+        <v>2.9</v>
+      </c>
+      <c r="AO308">
+        <v>2.7</v>
+      </c>
+      <c r="AP308">
+        <v>3.1</v>
+      </c>
+      <c r="AQ308">
+        <v>2.7</v>
+      </c>
+      <c r="AR308">
+        <v>2.5</v>
+      </c>
+      <c r="AS308">
+        <v>3.3</v>
+      </c>
+      <c r="AT308">
+        <v>2.88</v>
+      </c>
+      <c r="AU308">
+        <v>2.7</v>
+      </c>
+      <c r="AV308">
+        <v>3.3</v>
+      </c>
+      <c r="AW308">
+        <v>2.8</v>
+      </c>
+      <c r="AX308">
+        <v>2.4</v>
+      </c>
+      <c r="AY308">
+        <v>3.2</v>
+      </c>
+      <c r="AZ308">
+        <v>3</v>
+      </c>
+      <c r="BA308">
+        <v>39</v>
+      </c>
+      <c r="BB308">
+        <v>2.7</v>
+      </c>
+      <c r="BC308">
+        <v>2.56</v>
+      </c>
+      <c r="BD308">
+        <v>3.4</v>
+      </c>
+      <c r="BE308">
+        <v>3.25</v>
+      </c>
+      <c r="BF308">
+        <v>2.91</v>
+      </c>
+      <c r="BG308">
+        <v>2.78</v>
+      </c>
+      <c r="BH308">
+        <v>36</v>
+      </c>
+      <c r="BI308">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="BJ308">
+        <v>2.06</v>
+      </c>
+      <c r="BK308">
+        <v>1.81</v>
+      </c>
+      <c r="BL308">
+        <v>1.76</v>
+      </c>
+      <c r="BM308">
+        <v>23</v>
+      </c>
+      <c r="BN308">
+        <v>-0.25</v>
+      </c>
+      <c r="BO308">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="BP308">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="BQ308">
+        <v>1.74</v>
+      </c>
+      <c r="BR308">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="309" spans="1:70">
+      <c r="A309" t="s">
+        <v>70</v>
+      </c>
+      <c r="B309" s="1">
+        <v>41429</v>
+      </c>
+      <c r="C309" t="s">
+        <v>83</v>
+      </c>
+      <c r="D309" t="s">
+        <v>91</v>
+      </c>
+      <c r="E309">
+        <v>0</v>
+      </c>
+      <c r="F309">
+        <v>2</v>
+      </c>
+      <c r="G309" t="s">
+        <v>82</v>
+      </c>
+      <c r="H309">
+        <v>0</v>
+      </c>
+      <c r="I309">
+        <v>1</v>
+      </c>
+      <c r="J309" t="s">
+        <v>82</v>
+      </c>
+      <c r="K309">
+        <v>8</v>
+      </c>
+      <c r="L309">
+        <v>12</v>
+      </c>
+      <c r="M309">
+        <v>3</v>
+      </c>
+      <c r="N309">
+        <v>4</v>
+      </c>
+      <c r="O309">
+        <v>5</v>
+      </c>
+      <c r="P309">
+        <v>11</v>
+      </c>
+      <c r="Q309">
+        <v>8</v>
+      </c>
+      <c r="R309">
+        <v>4</v>
+      </c>
+      <c r="S309">
+        <v>0</v>
+      </c>
+      <c r="T309">
+        <v>0</v>
+      </c>
+      <c r="U309">
+        <v>0</v>
+      </c>
+      <c r="V309">
+        <v>0</v>
+      </c>
+      <c r="W309">
+        <v>3.3</v>
+      </c>
+      <c r="X309">
+        <v>3.6</v>
+      </c>
+      <c r="Y309">
+        <v>2.25</v>
+      </c>
+      <c r="Z309">
+        <v>3.3</v>
+      </c>
+      <c r="AA309">
+        <v>3.4</v>
+      </c>
+      <c r="AB309">
+        <v>2.15</v>
+      </c>
+      <c r="AC309">
+        <v>3.3</v>
+      </c>
+      <c r="AD309">
+        <v>3.4</v>
+      </c>
+      <c r="AE309">
+        <v>2.15</v>
+      </c>
+      <c r="AF309">
+        <v>3.1</v>
+      </c>
+      <c r="AG309">
+        <v>3.3</v>
+      </c>
+      <c r="AH309">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AI309">
+        <v>3</v>
+      </c>
+      <c r="AJ309">
+        <v>3.5</v>
+      </c>
+      <c r="AK309">
+        <v>2.25</v>
+      </c>
+      <c r="AL309">
+        <v>3.44</v>
+      </c>
+      <c r="AM309">
+        <v>3.61</v>
+      </c>
+      <c r="AN309">
+        <v>2.21</v>
+      </c>
+      <c r="AO309">
+        <v>3.3</v>
+      </c>
+      <c r="AP309">
+        <v>3.2</v>
+      </c>
+      <c r="AQ309">
+        <v>2.25</v>
+      </c>
+      <c r="AR309">
+        <v>3.2</v>
+      </c>
+      <c r="AS309">
+        <v>3.5</v>
+      </c>
+      <c r="AT309">
+        <v>2.25</v>
+      </c>
+      <c r="AU309">
+        <v>3.2</v>
+      </c>
+      <c r="AV309">
+        <v>3.6</v>
+      </c>
+      <c r="AW309">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AX309">
+        <v>3</v>
+      </c>
+      <c r="AY309">
+        <v>3.5</v>
+      </c>
+      <c r="AZ309">
+        <v>2.25</v>
+      </c>
+      <c r="BA309">
+        <v>39</v>
+      </c>
+      <c r="BB309">
+        <v>3.43</v>
+      </c>
+      <c r="BC309">
+        <v>3.19</v>
+      </c>
+      <c r="BD309">
+        <v>3.6</v>
+      </c>
+      <c r="BE309">
+        <v>3.45</v>
+      </c>
+      <c r="BF309">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="BG309">
+        <v>2.21</v>
+      </c>
+      <c r="BH309">
+        <v>34</v>
+      </c>
+      <c r="BI309">
+        <v>1.78</v>
+      </c>
+      <c r="BJ309">
+        <v>1.7</v>
+      </c>
+      <c r="BK309">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="BL309">
+        <v>2.12</v>
+      </c>
+      <c r="BM309">
+        <v>24</v>
+      </c>
+      <c r="BN309">
+        <v>0.25</v>
+      </c>
+      <c r="BO309">
+        <v>2.02</v>
+      </c>
+      <c r="BP309">
+        <v>1.96</v>
+      </c>
+      <c r="BQ309">
+        <v>1.95</v>
+      </c>
+      <c r="BR309">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="310" spans="1:70">
+      <c r="A310" t="s">
+        <v>70</v>
+      </c>
+      <c r="B310" s="1">
+        <v>41429</v>
+      </c>
+      <c r="C310" t="s">
+        <v>84</v>
+      </c>
+      <c r="D310" t="s">
+        <v>88</v>
+      </c>
+      <c r="E310">
+        <v>1</v>
+      </c>
+      <c r="F310">
+        <v>3</v>
+      </c>
+      <c r="G310" t="s">
+        <v>82</v>
+      </c>
+      <c r="H310">
+        <v>0</v>
+      </c>
+      <c r="I310">
+        <v>1</v>
+      </c>
+      <c r="J310" t="s">
+        <v>82</v>
+      </c>
+      <c r="K310">
+        <v>6</v>
+      </c>
+      <c r="L310">
+        <v>11</v>
+      </c>
+      <c r="M310">
+        <v>2</v>
+      </c>
+      <c r="N310">
+        <v>8</v>
+      </c>
+      <c r="O310">
+        <v>16</v>
+      </c>
+      <c r="P310">
+        <v>11</v>
+      </c>
+      <c r="Q310">
+        <v>4</v>
+      </c>
+      <c r="R310">
+        <v>2</v>
+      </c>
+      <c r="S310">
+        <v>3</v>
+      </c>
+      <c r="T310">
+        <v>1</v>
+      </c>
+      <c r="U310">
+        <v>0</v>
+      </c>
+      <c r="V310">
+        <v>0</v>
+      </c>
+      <c r="W310">
+        <v>2.1</v>
+      </c>
+      <c r="X310">
+        <v>3.4</v>
+      </c>
+      <c r="Y310">
+        <v>4</v>
+      </c>
+      <c r="Z310">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AA310">
+        <v>3.2</v>
+      </c>
+      <c r="AB310">
+        <v>3.8</v>
+      </c>
+      <c r="AC310">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AD310">
+        <v>3.2</v>
+      </c>
+      <c r="AE310">
+        <v>3.8</v>
+      </c>
+      <c r="AF310">
+        <v>2</v>
+      </c>
+      <c r="AG310">
+        <v>3.3</v>
+      </c>
+      <c r="AH310">
+        <v>3.6</v>
+      </c>
+      <c r="AI310">
+        <v>2.1</v>
+      </c>
+      <c r="AJ310">
+        <v>3.3</v>
+      </c>
+      <c r="AK310">
+        <v>3.5</v>
+      </c>
+      <c r="AL310">
+        <v>2.09</v>
+      </c>
+      <c r="AM310">
+        <v>3.35</v>
+      </c>
+      <c r="AN310">
+        <v>4.12</v>
+      </c>
+      <c r="AO310">
+        <v>2.15</v>
+      </c>
+      <c r="AP310">
+        <v>3.2</v>
+      </c>
+      <c r="AQ310">
+        <v>3.5</v>
+      </c>
+      <c r="AR310">
+        <v>2.1</v>
+      </c>
+      <c r="AS310">
+        <v>3.3</v>
+      </c>
+      <c r="AT310">
+        <v>3.6</v>
+      </c>
+      <c r="AU310">
+        <v>2.15</v>
+      </c>
+      <c r="AV310">
+        <v>3.3</v>
+      </c>
+      <c r="AW310">
+        <v>3.8</v>
+      </c>
+      <c r="AX310">
+        <v>2</v>
+      </c>
+      <c r="AY310">
+        <v>3.2</v>
+      </c>
+      <c r="AZ310">
+        <v>4</v>
+      </c>
+      <c r="BA310">
+        <v>39</v>
+      </c>
+      <c r="BB310">
+        <v>2.14</v>
+      </c>
+      <c r="BC310">
+        <v>2.06</v>
+      </c>
+      <c r="BD310">
+        <v>3.5</v>
+      </c>
+      <c r="BE310">
+        <v>3.28</v>
+      </c>
+      <c r="BF310">
+        <v>4.05</v>
+      </c>
+      <c r="BG310">
+        <v>3.74</v>
+      </c>
+      <c r="BH310">
+        <v>34</v>
+      </c>
+      <c r="BI310">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="BJ310">
+        <v>2.19</v>
+      </c>
+      <c r="BK310">
+        <v>1.72</v>
+      </c>
+      <c r="BL310">
+        <v>1.66</v>
+      </c>
+      <c r="BM310">
+        <v>22</v>
+      </c>
+      <c r="BN310">
+        <v>-0.25</v>
+      </c>
+      <c r="BO310">
+        <v>1.81</v>
+      </c>
+      <c r="BP310">
+        <v>1.77</v>
+      </c>
+      <c r="BQ310">
+        <v>2.16</v>
+      </c>
+      <c r="BR310">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="311" spans="1:70">
+      <c r="A311" t="s">
+        <v>70</v>
+      </c>
+      <c r="B311" s="1">
+        <v>41429</v>
+      </c>
+      <c r="C311" t="s">
+        <v>85</v>
+      </c>
+      <c r="D311" t="s">
+        <v>72</v>
+      </c>
+      <c r="E311">
+        <v>1</v>
+      </c>
+      <c r="F311">
+        <v>2</v>
+      </c>
+      <c r="G311" t="s">
+        <v>82</v>
+      </c>
+      <c r="H311">
+        <v>0</v>
+      </c>
+      <c r="I311">
+        <v>1</v>
+      </c>
+      <c r="J311" t="s">
+        <v>82</v>
+      </c>
+      <c r="K311">
+        <v>16</v>
+      </c>
+      <c r="L311">
+        <v>11</v>
+      </c>
+      <c r="M311">
+        <v>5</v>
+      </c>
+      <c r="N311">
+        <v>6</v>
+      </c>
+      <c r="O311">
+        <v>7</v>
+      </c>
+      <c r="P311">
+        <v>15</v>
+      </c>
+      <c r="Q311">
+        <v>6</v>
+      </c>
+      <c r="R311">
+        <v>4</v>
+      </c>
+      <c r="S311">
+        <v>2</v>
+      </c>
+      <c r="T311">
+        <v>4</v>
+      </c>
+      <c r="U311">
+        <v>0</v>
+      </c>
+      <c r="V311">
+        <v>1</v>
+      </c>
+      <c r="W311">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="X311">
+        <v>3.7</v>
+      </c>
+      <c r="Y311">
+        <v>1.95</v>
+      </c>
+      <c r="Z311">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AA311">
+        <v>3.5</v>
+      </c>
+      <c r="AB311">
+        <v>1.87</v>
+      </c>
+      <c r="AC311">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AD311">
+        <v>3.5</v>
+      </c>
+      <c r="AE311">
+        <v>1.87</v>
+      </c>
+      <c r="AF311">
+        <v>3.8</v>
+      </c>
+      <c r="AG311">
+        <v>3.45</v>
+      </c>
+      <c r="AH311">
+        <v>1.9</v>
+      </c>
+      <c r="AI311">
+        <v>4</v>
+      </c>
+      <c r="AJ311">
+        <v>3.5</v>
+      </c>
+      <c r="AK311">
+        <v>1.9</v>
+      </c>
+      <c r="AL311">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="AM311">
+        <v>3.69</v>
+      </c>
+      <c r="AN311">
+        <v>1.96</v>
+      </c>
+      <c r="AO311">
+        <v>4</v>
+      </c>
+      <c r="AP311">
+        <v>3.3</v>
+      </c>
+      <c r="AQ311">
+        <v>1.95</v>
+      </c>
+      <c r="AR311">
+        <v>4</v>
+      </c>
+      <c r="AS311">
+        <v>3.75</v>
+      </c>
+      <c r="AT311">
+        <v>1.91</v>
+      </c>
+      <c r="AU311">
+        <v>3.9</v>
+      </c>
+      <c r="AV311">
+        <v>3.75</v>
+      </c>
+      <c r="AW311">
+        <v>2</v>
+      </c>
+      <c r="AX311">
+        <v>3.8</v>
+      </c>
+      <c r="AY311">
+        <v>3.5</v>
+      </c>
+      <c r="AZ311">
+        <v>1.91</v>
+      </c>
+      <c r="BA311">
+        <v>39</v>
+      </c>
+      <c r="BB311">
+        <v>4.33</v>
+      </c>
+      <c r="BC311">
+        <v>3.93</v>
+      </c>
+      <c r="BD311">
+        <v>3.75</v>
+      </c>
+      <c r="BE311">
+        <v>3.51</v>
+      </c>
+      <c r="BF311">
+        <v>2</v>
+      </c>
+      <c r="BG311">
+        <v>1.93</v>
+      </c>
+      <c r="BH311">
+        <v>36</v>
+      </c>
+      <c r="BI311">
+        <v>1.78</v>
+      </c>
+      <c r="BJ311">
+        <v>1.73</v>
+      </c>
+      <c r="BK311">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="BL311">
+        <v>2.1</v>
+      </c>
+      <c r="BM311">
+        <v>24</v>
+      </c>
+      <c r="BN311">
+        <v>0.25</v>
+      </c>
+      <c r="BO311">
+        <v>2.33</v>
+      </c>
+      <c r="BP311">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="BQ311">
+        <v>1.74</v>
+      </c>
+      <c r="BR311">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="312" spans="1:70">
+      <c r="A312" t="s">
+        <v>70</v>
+      </c>
+      <c r="B312" s="1">
+        <v>41459</v>
+      </c>
+      <c r="C312" t="s">
+        <v>93</v>
+      </c>
+      <c r="D312" t="s">
+        <v>73</v>
+      </c>
+      <c r="E312">
+        <v>2</v>
+      </c>
+      <c r="F312">
+        <v>1</v>
+      </c>
+      <c r="G312" t="s">
+        <v>77</v>
+      </c>
+      <c r="H312">
+        <v>0</v>
+      </c>
+      <c r="I312">
+        <v>1</v>
+      </c>
+      <c r="J312" t="s">
+        <v>82</v>
+      </c>
+      <c r="K312">
+        <v>14</v>
+      </c>
+      <c r="L312">
+        <v>7</v>
+      </c>
+      <c r="M312">
+        <v>7</v>
+      </c>
+      <c r="N312">
+        <v>3</v>
+      </c>
+      <c r="O312">
+        <v>9</v>
+      </c>
+      <c r="P312">
+        <v>15</v>
+      </c>
+      <c r="Q312">
+        <v>8</v>
+      </c>
+      <c r="R312">
+        <v>5</v>
+      </c>
+      <c r="S312">
+        <v>0</v>
+      </c>
+      <c r="T312">
+        <v>2</v>
+      </c>
+      <c r="U312">
+        <v>0</v>
+      </c>
+      <c r="V312">
+        <v>0</v>
+      </c>
+      <c r="W312">
+        <v>1.36</v>
+      </c>
+      <c r="X312">
+        <v>5</v>
+      </c>
+      <c r="Y312">
+        <v>11</v>
+      </c>
+      <c r="Z312">
+        <v>1.3</v>
+      </c>
+      <c r="AA312">
+        <v>5</v>
+      </c>
+      <c r="AB312">
+        <v>10.5</v>
+      </c>
+      <c r="AC312">
+        <v>1.3</v>
+      </c>
+      <c r="AD312">
+        <v>5</v>
+      </c>
+      <c r="AE312">
+        <v>10.5</v>
+      </c>
+      <c r="AF312">
+        <v>1.33</v>
+      </c>
+      <c r="AG312">
+        <v>4.8</v>
+      </c>
+      <c r="AH312">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="AI312">
+        <v>1.33</v>
+      </c>
+      <c r="AJ312">
+        <v>5</v>
+      </c>
+      <c r="AK312">
+        <v>9</v>
+      </c>
+      <c r="AL312">
+        <v>1.34</v>
+      </c>
+      <c r="AM312">
+        <v>5.42</v>
+      </c>
+      <c r="AN312">
+        <v>11.3</v>
+      </c>
+      <c r="AO312">
+        <v>1.33</v>
+      </c>
+      <c r="AP312">
+        <v>4.5</v>
+      </c>
+      <c r="AQ312">
+        <v>11</v>
+      </c>
+      <c r="AR312">
+        <v>1.33</v>
+      </c>
+      <c r="AS312">
+        <v>5</v>
+      </c>
+      <c r="AT312">
+        <v>10</v>
+      </c>
+      <c r="AU312">
+        <v>1.36</v>
+      </c>
+      <c r="AV312">
+        <v>5.2</v>
+      </c>
+      <c r="AW312">
+        <v>10</v>
+      </c>
+      <c r="AX312">
+        <v>1.33</v>
+      </c>
+      <c r="AY312">
+        <v>5</v>
+      </c>
+      <c r="AZ312">
+        <v>9</v>
+      </c>
+      <c r="BA312">
+        <v>39</v>
+      </c>
+      <c r="BB312">
+        <v>1.36</v>
+      </c>
+      <c r="BC312">
+        <v>1.33</v>
+      </c>
+      <c r="BD312">
+        <v>5.41</v>
+      </c>
+      <c r="BE312">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="BF312">
+        <v>11</v>
+      </c>
+      <c r="BG312">
+        <v>9.82</v>
+      </c>
+      <c r="BH312">
+        <v>34</v>
+      </c>
+      <c r="BI312">
+        <v>1.74</v>
+      </c>
+      <c r="BJ312">
+        <v>1.68</v>
+      </c>
+      <c r="BK312">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="BL312">
+        <v>2.15</v>
+      </c>
+      <c r="BM312">
+        <v>23</v>
+      </c>
+      <c r="BN312">
+        <v>-1.5</v>
+      </c>
+      <c r="BO312">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BP312">
+        <v>1.96</v>
+      </c>
+      <c r="BQ312">
+        <v>1.94</v>
+      </c>
+      <c r="BR312">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="313" spans="1:70">
+      <c r="A313" t="s">
+        <v>70</v>
+      </c>
+      <c r="B313" s="1">
+        <v>41459</v>
+      </c>
+      <c r="C313" t="s">
+        <v>86</v>
+      </c>
+      <c r="D313" t="s">
+        <v>87</v>
+      </c>
+      <c r="E313">
+        <v>0</v>
+      </c>
+      <c r="F313">
+        <v>0</v>
+      </c>
+      <c r="G313" t="s">
+        <v>74</v>
+      </c>
+      <c r="H313">
+        <v>0</v>
+      </c>
+      <c r="I313">
+        <v>0</v>
+      </c>
+      <c r="J313" t="s">
+        <v>74</v>
+      </c>
+      <c r="K313">
+        <v>19</v>
+      </c>
+      <c r="L313">
+        <v>10</v>
+      </c>
+      <c r="M313">
+        <v>12</v>
+      </c>
+      <c r="N313">
+        <v>4</v>
+      </c>
+      <c r="O313">
+        <v>8</v>
+      </c>
+      <c r="P313">
+        <v>4</v>
+      </c>
+      <c r="Q313">
+        <v>12</v>
+      </c>
+      <c r="R313">
+        <v>2</v>
+      </c>
+      <c r="S313">
+        <v>0</v>
+      </c>
+      <c r="T313">
+        <v>1</v>
+      </c>
+      <c r="U313">
+        <v>0</v>
+      </c>
+      <c r="V313">
+        <v>0</v>
+      </c>
+      <c r="W313">
+        <v>1.36</v>
+      </c>
+      <c r="X313">
+        <v>5.5</v>
+      </c>
+      <c r="Y313">
+        <v>9</v>
+      </c>
+      <c r="Z313">
+        <v>1.35</v>
+      </c>
+      <c r="AA313">
+        <v>5</v>
+      </c>
+      <c r="AB313">
+        <v>8</v>
+      </c>
+      <c r="AC313">
+        <v>1.35</v>
+      </c>
+      <c r="AD313">
+        <v>5</v>
+      </c>
+      <c r="AE313">
+        <v>8</v>
+      </c>
+      <c r="AF313">
+        <v>1.35</v>
+      </c>
+      <c r="AG313">
+        <v>4.8</v>
+      </c>
+      <c r="AH313">
+        <v>7.6</v>
+      </c>
+      <c r="AI313">
+        <v>1.36</v>
+      </c>
+      <c r="AJ313">
+        <v>5</v>
+      </c>
+      <c r="AK313">
+        <v>7.5</v>
+      </c>
+      <c r="AL313">
+        <v>1.35</v>
+      </c>
+      <c r="AM313">
+        <v>5.5</v>
+      </c>
+      <c r="AN313">
+        <v>10.02</v>
+      </c>
+      <c r="AO313">
+        <v>1.36</v>
+      </c>
+      <c r="AP313">
+        <v>5</v>
+      </c>
+      <c r="AQ313">
+        <v>8</v>
+      </c>
+      <c r="AR313">
+        <v>1.33</v>
+      </c>
+      <c r="AS313">
+        <v>5</v>
+      </c>
+      <c r="AT313">
+        <v>9.5</v>
+      </c>
+      <c r="AU313">
+        <v>1.36</v>
+      </c>
+      <c r="AV313">
+        <v>5.4</v>
+      </c>
+      <c r="AW313">
+        <v>9.5</v>
+      </c>
+      <c r="AX313">
+        <v>1.33</v>
+      </c>
+      <c r="AY313">
+        <v>5</v>
+      </c>
+      <c r="AZ313">
+        <v>9</v>
+      </c>
+      <c r="BA313">
+        <v>39</v>
+      </c>
+      <c r="BB313">
+        <v>1.37</v>
+      </c>
+      <c r="BC313">
+        <v>1.34</v>
+      </c>
+      <c r="BD313">
+        <v>5.5</v>
+      </c>
+      <c r="BE313">
+        <v>5.01</v>
+      </c>
+      <c r="BF313">
+        <v>10</v>
+      </c>
+      <c r="BG313">
+        <v>8.99</v>
+      </c>
+      <c r="BH313">
+        <v>25</v>
+      </c>
+      <c r="BI313">
+        <v>1.6</v>
+      </c>
+      <c r="BJ313">
+        <v>1.55</v>
+      </c>
+      <c r="BK313">
+        <v>2.56</v>
+      </c>
+      <c r="BL313">
+        <v>2.37</v>
+      </c>
+      <c r="BM313">
+        <v>25</v>
+      </c>
+      <c r="BN313">
+        <v>-1.5</v>
+      </c>
+      <c r="BO313">
+        <v>1.99</v>
+      </c>
+      <c r="BP313">
+        <v>1.94</v>
+      </c>
+      <c r="BQ313">
+        <v>1.96</v>
+      </c>
+      <c r="BR313">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="314" spans="1:70">
+      <c r="A314" t="s">
+        <v>70</v>
+      </c>
+      <c r="B314" s="1">
+        <v>41459</v>
+      </c>
+      <c r="C314" t="s">
+        <v>78</v>
+      </c>
+      <c r="D314" t="s">
+        <v>75</v>
+      </c>
+      <c r="E314">
+        <v>1</v>
+      </c>
+      <c r="F314">
+        <v>0</v>
+      </c>
+      <c r="G314" t="s">
+        <v>77</v>
+      </c>
+      <c r="H314">
+        <v>0</v>
+      </c>
+      <c r="I314">
+        <v>0</v>
+      </c>
+      <c r="J314" t="s">
+        <v>74</v>
+      </c>
+      <c r="K314">
+        <v>20</v>
+      </c>
+      <c r="L314">
+        <v>5</v>
+      </c>
+      <c r="M314">
+        <v>10</v>
+      </c>
+      <c r="N314">
+        <v>3</v>
+      </c>
+      <c r="O314">
+        <v>13</v>
+      </c>
+      <c r="P314">
+        <v>11</v>
+      </c>
+      <c r="Q314">
+        <v>10</v>
+      </c>
+      <c r="R314">
+        <v>3</v>
+      </c>
+      <c r="S314">
+        <v>2</v>
+      </c>
+      <c r="T314">
+        <v>2</v>
+      </c>
+      <c r="U314">
+        <v>0</v>
+      </c>
+      <c r="V314">
+        <v>0</v>
+      </c>
+      <c r="W314">
+        <v>2.1</v>
+      </c>
+      <c r="X314">
+        <v>3.5</v>
+      </c>
+      <c r="Y314">
+        <v>3.8</v>
+      </c>
+      <c r="Z314">
+        <v>2</v>
+      </c>
+      <c r="AA314">
+        <v>3.25</v>
+      </c>
+      <c r="AB314">
+        <v>3.9</v>
+      </c>
+      <c r="AC314">
+        <v>2</v>
+      </c>
+      <c r="AD314">
+        <v>3.25</v>
+      </c>
+      <c r="AE314">
+        <v>3.9</v>
+      </c>
+      <c r="AF314">
+        <v>1.95</v>
+      </c>
+      <c r="AG314">
+        <v>3.4</v>
+      </c>
+      <c r="AH314">
+        <v>3.6</v>
+      </c>
+      <c r="AI314">
+        <v>2.1</v>
+      </c>
+      <c r="AJ314">
+        <v>3.4</v>
+      </c>
+      <c r="AK314">
+        <v>3.4</v>
+      </c>
+      <c r="AL314">
+        <v>2.11</v>
+      </c>
+      <c r="AM314">
+        <v>3.51</v>
+      </c>
+      <c r="AN314">
+        <v>3.83</v>
+      </c>
+      <c r="AO314">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AP314">
+        <v>3.4</v>
+      </c>
+      <c r="AQ314">
+        <v>3.6</v>
+      </c>
+      <c r="AR314">
+        <v>2.1</v>
+      </c>
+      <c r="AS314">
+        <v>3.4</v>
+      </c>
+      <c r="AT314">
+        <v>3.6</v>
+      </c>
+      <c r="AU314">
+        <v>2.15</v>
+      </c>
+      <c r="AV314">
+        <v>3.6</v>
+      </c>
+      <c r="AW314">
+        <v>3.5</v>
+      </c>
+      <c r="AX314">
+        <v>2</v>
+      </c>
+      <c r="AY314">
+        <v>3.4</v>
+      </c>
+      <c r="AZ314">
+        <v>3.75</v>
+      </c>
+      <c r="BA314">
+        <v>39</v>
+      </c>
+      <c r="BB314">
+        <v>2.1</v>
+      </c>
+      <c r="BC314">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="BD314">
+        <v>3.55</v>
+      </c>
+      <c r="BE314">
+        <v>3.4</v>
+      </c>
+      <c r="BF314">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="BG314">
+        <v>3.73</v>
+      </c>
+      <c r="BH314">
+        <v>34</v>
+      </c>
+      <c r="BI314">
+        <v>1.89</v>
+      </c>
+      <c r="BJ314">
+        <v>1.81</v>
+      </c>
+      <c r="BK314">
+        <v>2.09</v>
+      </c>
+      <c r="BL314">
+        <v>1.98</v>
+      </c>
+      <c r="BM314">
+        <v>22</v>
+      </c>
+      <c r="BN314">
+        <v>-0.25</v>
+      </c>
+      <c r="BO314">
+        <v>1.8</v>
+      </c>
+      <c r="BP314">
+        <v>1.72</v>
+      </c>
+      <c r="BQ314">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="BR314">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="315" spans="1:70">
+      <c r="A315" t="s">
+        <v>70</v>
+      </c>
+      <c r="B315" s="1">
+        <v>41459</v>
+      </c>
+      <c r="C315" t="s">
+        <v>80</v>
+      </c>
+      <c r="D315" t="s">
+        <v>92</v>
+      </c>
+      <c r="E315">
+        <v>1</v>
+      </c>
+      <c r="F315">
+        <v>1</v>
+      </c>
+      <c r="G315" t="s">
+        <v>74</v>
+      </c>
+      <c r="H315">
+        <v>0</v>
+      </c>
+      <c r="I315">
+        <v>0</v>
+      </c>
+      <c r="J315" t="s">
+        <v>74</v>
+      </c>
+      <c r="K315">
+        <v>6</v>
+      </c>
+      <c r="L315">
+        <v>16</v>
+      </c>
+      <c r="M315">
+        <v>2</v>
+      </c>
+      <c r="N315">
+        <v>10</v>
+      </c>
+      <c r="O315">
+        <v>9</v>
+      </c>
+      <c r="P315">
+        <v>12</v>
+      </c>
+      <c r="Q315">
+        <v>2</v>
+      </c>
+      <c r="R315">
+        <v>10</v>
+      </c>
+      <c r="S315">
+        <v>2</v>
+      </c>
+      <c r="T315">
+        <v>3</v>
+      </c>
+      <c r="U315">
+        <v>1</v>
+      </c>
+      <c r="V315">
+        <v>0</v>
+      </c>
+      <c r="W315">
+        <v>2.38</v>
+      </c>
+      <c r="X315">
+        <v>3.4</v>
+      </c>
+      <c r="Y315">
+        <v>3.25</v>
+      </c>
+      <c r="Z315">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA315">
+        <v>3.25</v>
+      </c>
+      <c r="AB315">
+        <v>3.1</v>
+      </c>
+      <c r="AC315">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AD315">
+        <v>3.25</v>
+      </c>
+      <c r="AE315">
+        <v>3.1</v>
+      </c>
+      <c r="AF315">
+        <v>2.4</v>
+      </c>
+      <c r="AG315">
+        <v>3.3</v>
+      </c>
+      <c r="AH315">
+        <v>2.75</v>
+      </c>
+      <c r="AI315">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AJ315">
+        <v>3.4</v>
+      </c>
+      <c r="AK315">
+        <v>3</v>
+      </c>
+      <c r="AL315">
+        <v>2.39</v>
+      </c>
+      <c r="AM315">
+        <v>3.41</v>
+      </c>
+      <c r="AN315">
+        <v>3.24</v>
+      </c>
+      <c r="AO315">
+        <v>2.4</v>
+      </c>
+      <c r="AP315">
+        <v>3.1</v>
+      </c>
+      <c r="AQ315">
+        <v>3.1</v>
+      </c>
+      <c r="AR315">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AS315">
+        <v>3.4</v>
+      </c>
+      <c r="AT315">
+        <v>3.2</v>
+      </c>
+      <c r="AU315">
+        <v>2.4</v>
+      </c>
+      <c r="AV315">
+        <v>3.4</v>
+      </c>
+      <c r="AW315">
+        <v>3.12</v>
+      </c>
+      <c r="AX315">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AY315">
+        <v>3.4</v>
+      </c>
+      <c r="AZ315">
+        <v>3</v>
+      </c>
+      <c r="BA315">
+        <v>39</v>
+      </c>
+      <c r="BB315">
+        <v>2.42</v>
+      </c>
+      <c r="BC315">
+        <v>2.34</v>
+      </c>
+      <c r="BD315">
+        <v>3.45</v>
+      </c>
+      <c r="BE315">
+        <v>3.34</v>
+      </c>
+      <c r="BF315">
+        <v>3.25</v>
+      </c>
+      <c r="BG315">
+        <v>3.03</v>
+      </c>
+      <c r="BH315">
+        <v>36</v>
+      </c>
+      <c r="BI315">
+        <v>1.95</v>
+      </c>
+      <c r="BJ315">
+        <v>1.85</v>
+      </c>
+      <c r="BK315">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="BL315">
+        <v>1.95</v>
+      </c>
+      <c r="BM315">
+        <v>24</v>
+      </c>
+      <c r="BN315">
+        <v>-0.25</v>
+      </c>
+      <c r="BO315">
+        <v>2.08</v>
+      </c>
+      <c r="BP315">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BQ315">
+        <v>1.89</v>
+      </c>
+      <c r="BR315">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="316" spans="1:70">
+      <c r="A316" t="s">
+        <v>70</v>
+      </c>
+      <c r="B316" s="1">
+        <v>41459</v>
+      </c>
+      <c r="C316" t="s">
+        <v>79</v>
+      </c>
+      <c r="D316" t="s">
+        <v>95</v>
+      </c>
+      <c r="E316">
+        <v>2</v>
+      </c>
+      <c r="F316">
+        <v>2</v>
+      </c>
+      <c r="G316" t="s">
+        <v>74</v>
+      </c>
+      <c r="H316">
+        <v>1</v>
+      </c>
+      <c r="I316">
+        <v>1</v>
+      </c>
+      <c r="J316" t="s">
+        <v>74</v>
+      </c>
+      <c r="K316">
+        <v>19</v>
+      </c>
+      <c r="L316">
+        <v>9</v>
+      </c>
+      <c r="M316">
+        <v>10</v>
+      </c>
+      <c r="N316">
+        <v>5</v>
+      </c>
+      <c r="O316">
+        <v>14</v>
+      </c>
+      <c r="P316">
+        <v>8</v>
+      </c>
+      <c r="Q316">
+        <v>7</v>
+      </c>
+      <c r="R316">
+        <v>6</v>
+      </c>
+      <c r="S316">
+        <v>1</v>
+      </c>
+      <c r="T316">
+        <v>1</v>
+      </c>
+      <c r="U316">
+        <v>0</v>
+      </c>
+      <c r="V316">
+        <v>0</v>
+      </c>
+      <c r="W316">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X316">
+        <v>3.4</v>
+      </c>
+      <c r="Y316">
+        <v>3.6</v>
+      </c>
+      <c r="Z316">
+        <v>2.25</v>
+      </c>
+      <c r="AA316">
+        <v>3.25</v>
+      </c>
+      <c r="AB316">
+        <v>3.2</v>
+      </c>
+      <c r="AC316">
+        <v>2.25</v>
+      </c>
+      <c r="AD316">
+        <v>3.25</v>
+      </c>
+      <c r="AE316">
+        <v>3.2</v>
+      </c>
+      <c r="AF316">
+        <v>2.1</v>
+      </c>
+      <c r="AG316">
+        <v>3.3</v>
+      </c>
+      <c r="AH316">
+        <v>3.3</v>
+      </c>
+      <c r="AI316">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AJ316">
+        <v>3.3</v>
+      </c>
+      <c r="AK316">
+        <v>3.2</v>
+      </c>
+      <c r="AL316">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AM316">
+        <v>3.46</v>
+      </c>
+      <c r="AN316">
+        <v>3.61</v>
+      </c>
+      <c r="AO316">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AP316">
+        <v>3.2</v>
+      </c>
+      <c r="AQ316">
+        <v>3.4</v>
+      </c>
+      <c r="AR316">
+        <v>2.25</v>
+      </c>
+      <c r="AS316">
+        <v>3.3</v>
+      </c>
+      <c r="AT316">
+        <v>3.4</v>
+      </c>
+      <c r="AU316">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AV316">
+        <v>3.5</v>
+      </c>
+      <c r="AW316">
+        <v>3.3</v>
+      </c>
+      <c r="AX316">
+        <v>2.1</v>
+      </c>
+      <c r="AY316">
+        <v>3.4</v>
+      </c>
+      <c r="AZ316">
+        <v>3.3</v>
+      </c>
+      <c r="BA316">
+        <v>35</v>
+      </c>
+      <c r="BB316">
+        <v>2.25</v>
+      </c>
+      <c r="BC316">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="BD316">
+        <v>3.4</v>
+      </c>
+      <c r="BE316">
+        <v>3.26</v>
+      </c>
+      <c r="BF316">
+        <v>3.65</v>
+      </c>
+      <c r="BG316">
+        <v>3.42</v>
+      </c>
+      <c r="BH316">
+        <v>32</v>
+      </c>
+      <c r="BI316">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="BJ316">
+        <v>2.06</v>
+      </c>
+      <c r="BK316">
+        <v>1.81</v>
+      </c>
+      <c r="BL316">
+        <v>1.74</v>
+      </c>
+      <c r="BM316">
+        <v>19</v>
+      </c>
+      <c r="BN316">
+        <v>-0.25</v>
+      </c>
+      <c r="BO316">
+        <v>1.93</v>
+      </c>
+      <c r="BP316">
+        <v>1.87</v>
+      </c>
+      <c r="BQ316">
+        <v>2.04</v>
+      </c>
+      <c r="BR316">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="317" spans="1:70">
+      <c r="A317" t="s">
+        <v>70</v>
+      </c>
+      <c r="B317" s="1">
+        <v>41490</v>
+      </c>
+      <c r="C317" t="s">
+        <v>96</v>
+      </c>
+      <c r="D317" t="s">
+        <v>90</v>
+      </c>
+      <c r="E317">
+        <v>1</v>
+      </c>
+      <c r="F317">
+        <v>2</v>
+      </c>
+      <c r="G317" t="s">
+        <v>82</v>
+      </c>
+      <c r="H317">
+        <v>0</v>
+      </c>
+      <c r="I317">
+        <v>0</v>
+      </c>
+      <c r="J317" t="s">
+        <v>74</v>
+      </c>
+      <c r="K317">
+        <v>16</v>
+      </c>
+      <c r="L317">
+        <v>9</v>
+      </c>
+      <c r="M317">
+        <v>7</v>
+      </c>
+      <c r="N317">
+        <v>5</v>
+      </c>
+      <c r="O317">
+        <v>13</v>
+      </c>
+      <c r="P317">
+        <v>18</v>
+      </c>
+      <c r="Q317">
+        <v>9</v>
+      </c>
+      <c r="R317">
+        <v>4</v>
+      </c>
+      <c r="S317">
+        <v>3</v>
+      </c>
+      <c r="T317">
+        <v>5</v>
+      </c>
+      <c r="U317">
+        <v>0</v>
+      </c>
+      <c r="V317">
+        <v>0</v>
+      </c>
+      <c r="W317">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X317">
+        <v>3.5</v>
+      </c>
+      <c r="Y317">
+        <v>3.3</v>
+      </c>
+      <c r="Z317">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AA317">
+        <v>3.4</v>
+      </c>
+      <c r="AB317">
+        <v>3.2</v>
+      </c>
+      <c r="AC317">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AD317">
+        <v>3.4</v>
+      </c>
+      <c r="AE317">
+        <v>3.2</v>
+      </c>
+      <c r="AF317">
+        <v>2</v>
+      </c>
+      <c r="AG317">
+        <v>3.3</v>
+      </c>
+      <c r="AH317">
+        <v>3.6</v>
+      </c>
+      <c r="AI317">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AJ317">
+        <v>3.4</v>
+      </c>
+      <c r="AK317">
+        <v>3.2</v>
+      </c>
+      <c r="AL317">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="AM317">
+        <v>3.48</v>
+      </c>
+      <c r="AN317">
+        <v>3.5</v>
+      </c>
+      <c r="AO317">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AP317">
+        <v>3</v>
+      </c>
+      <c r="AQ317">
+        <v>3.4</v>
+      </c>
+      <c r="AR317">
+        <v>2.25</v>
+      </c>
+      <c r="AS317">
+        <v>3.5</v>
+      </c>
+      <c r="AT317">
+        <v>3.4</v>
+      </c>
+      <c r="AU317">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AV317">
+        <v>3.5</v>
+      </c>
+      <c r="AW317">
+        <v>3.3</v>
+      </c>
+      <c r="AX317">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AY317">
+        <v>3.4</v>
+      </c>
+      <c r="AZ317">
+        <v>3.4</v>
+      </c>
+      <c r="BA317">
+        <v>37</v>
+      </c>
+      <c r="BB317">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="BC317">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BD317">
+        <v>3.52</v>
+      </c>
+      <c r="BE317">
+        <v>3.32</v>
+      </c>
+      <c r="BF317">
+        <v>3.6</v>
+      </c>
+      <c r="BG317">
+        <v>3.33</v>
+      </c>
+      <c r="BH317">
+        <v>34</v>
+      </c>
+      <c r="BI317">
+        <v>1.83</v>
+      </c>
+      <c r="BJ317">
+        <v>1.75</v>
+      </c>
+      <c r="BK317">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BL317">
+        <v>2.06</v>
+      </c>
+      <c r="BM317">
+        <v>22</v>
+      </c>
+      <c r="BN317">
+        <v>-0.25</v>
+      </c>
+      <c r="BO317">
+        <v>1.92</v>
+      </c>
+      <c r="BP317">
+        <v>1.89</v>
+      </c>
+      <c r="BQ317">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BR317">
+        <v>1.98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>